<commit_message>
LAB 3-3 to 3-4 UPDATE
</commit_message>
<xml_diff>
--- a/Lab 03/diglab_03_03/diglab_03_03_pics/diglab_03_03_table.xlsx
+++ b/Lab 03/diglab_03_03/diglab_03_03_pics/diglab_03_03_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\College Year 2\2110263 DIG LOGIC LAB I\2110263-DIG-LOGIC-LAB-I\Lab 03\diglab_03_03\diglab_03_03_pics\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30613701-FD57-42D7-9810-B97CC14E2C61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0F0B0FB-A7B4-4A31-A5B2-326BB44F03D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{E2F5C648-1E30-482C-A813-F5047B4D4EC4}"/>
   </bookViews>
@@ -182,9 +182,6 @@
     <t>S1S0'C3</t>
   </si>
   <si>
-    <t>S1S0D4</t>
-  </si>
-  <si>
     <t>Z0</t>
   </si>
   <si>
@@ -210,6 +207,9 @@
   </si>
   <si>
     <t>6 4 2 -3 Code</t>
+  </si>
+  <si>
+    <t>S1S0D3</t>
   </si>
 </sst>
 </file>
@@ -771,7 +771,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -887,9 +887,48 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -908,18 +947,6 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -927,36 +954,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1287,62 +1284,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="59" t="s">
+      <c r="A1" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
+      <c r="K1" s="49"/>
+      <c r="L1" s="49"/>
+      <c r="M1" s="49"/>
+      <c r="N1" s="49"/>
+      <c r="O1" s="49"/>
+      <c r="P1" s="49"/>
+      <c r="Q1" s="49"/>
+      <c r="R1" s="49"/>
+      <c r="S1" s="49"/>
+      <c r="T1" s="49"/>
+      <c r="U1" s="50"/>
+    </row>
+    <row r="2" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="39" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="40"/>
+      <c r="L2" s="40"/>
+      <c r="M2" s="41"/>
+      <c r="N2" s="39" t="s">
         <v>55</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
-      <c r="L1" s="60"/>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="60"/>
-      <c r="Q1" s="60"/>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="61"/>
-    </row>
-    <row r="2" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="47" t="s">
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
+      <c r="Q2" s="41"/>
+      <c r="R2" s="39" t="s">
         <v>58</v>
       </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="47" t="s">
-        <v>57</v>
-      </c>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="47" t="s">
-        <v>56</v>
-      </c>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="47" t="s">
-        <v>59</v>
-      </c>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="49"/>
+      <c r="S2" s="40"/>
+      <c r="T2" s="40"/>
+      <c r="U2" s="41"/>
     </row>
     <row r="3" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
@@ -2075,30 +2072,30 @@
       <c r="E14" s="27">
         <v>0</v>
       </c>
-      <c r="F14" s="53" t="s">
+      <c r="F14" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="53" t="s">
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="K14" s="53"/>
-      <c r="L14" s="53"/>
-      <c r="M14" s="54"/>
-      <c r="N14" s="53" t="s">
+      <c r="K14" s="42"/>
+      <c r="L14" s="42"/>
+      <c r="M14" s="43"/>
+      <c r="N14" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="O14" s="53"/>
-      <c r="P14" s="53"/>
-      <c r="Q14" s="54"/>
-      <c r="R14" s="53" t="s">
+      <c r="O14" s="42"/>
+      <c r="P14" s="42"/>
+      <c r="Q14" s="43"/>
+      <c r="R14" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="S14" s="53"/>
-      <c r="T14" s="53"/>
-      <c r="U14" s="54"/>
+      <c r="S14" s="42"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="43"/>
     </row>
     <row r="15" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
@@ -2116,22 +2113,22 @@
       <c r="E15" s="24">
         <v>1</v>
       </c>
-      <c r="F15" s="62"/>
-      <c r="G15" s="62"/>
-      <c r="H15" s="62"/>
-      <c r="I15" s="56"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="62"/>
-      <c r="L15" s="62"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="62"/>
-      <c r="O15" s="62"/>
-      <c r="P15" s="62"/>
-      <c r="Q15" s="56"/>
-      <c r="R15" s="62"/>
-      <c r="S15" s="62"/>
-      <c r="T15" s="62"/>
-      <c r="U15" s="56"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="44"/>
+      <c r="K15" s="44"/>
+      <c r="L15" s="44"/>
+      <c r="M15" s="45"/>
+      <c r="N15" s="44"/>
+      <c r="O15" s="44"/>
+      <c r="P15" s="44"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="44"/>
+      <c r="S15" s="44"/>
+      <c r="T15" s="44"/>
+      <c r="U15" s="45"/>
     </row>
     <row r="16" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
@@ -2149,22 +2146,22 @@
       <c r="E16" s="24">
         <v>0</v>
       </c>
-      <c r="F16" s="62"/>
-      <c r="G16" s="62"/>
-      <c r="H16" s="62"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="62"/>
-      <c r="K16" s="62"/>
-      <c r="L16" s="62"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="62"/>
-      <c r="O16" s="62"/>
-      <c r="P16" s="62"/>
-      <c r="Q16" s="56"/>
-      <c r="R16" s="62"/>
-      <c r="S16" s="62"/>
-      <c r="T16" s="62"/>
-      <c r="U16" s="56"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
+      <c r="J16" s="44"/>
+      <c r="K16" s="44"/>
+      <c r="L16" s="44"/>
+      <c r="M16" s="45"/>
+      <c r="N16" s="44"/>
+      <c r="O16" s="44"/>
+      <c r="P16" s="44"/>
+      <c r="Q16" s="45"/>
+      <c r="R16" s="44"/>
+      <c r="S16" s="44"/>
+      <c r="T16" s="44"/>
+      <c r="U16" s="45"/>
     </row>
     <row r="17" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
@@ -2182,22 +2179,22 @@
       <c r="E17" s="24">
         <v>1</v>
       </c>
-      <c r="F17" s="62"/>
-      <c r="G17" s="62"/>
-      <c r="H17" s="62"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="62"/>
-      <c r="K17" s="62"/>
-      <c r="L17" s="62"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="62"/>
-      <c r="O17" s="62"/>
-      <c r="P17" s="62"/>
-      <c r="Q17" s="56"/>
-      <c r="R17" s="62"/>
-      <c r="S17" s="62"/>
-      <c r="T17" s="62"/>
-      <c r="U17" s="56"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
+      <c r="J17" s="44"/>
+      <c r="K17" s="44"/>
+      <c r="L17" s="44"/>
+      <c r="M17" s="45"/>
+      <c r="N17" s="44"/>
+      <c r="O17" s="44"/>
+      <c r="P17" s="44"/>
+      <c r="Q17" s="45"/>
+      <c r="R17" s="44"/>
+      <c r="S17" s="44"/>
+      <c r="T17" s="44"/>
+      <c r="U17" s="45"/>
     </row>
     <row r="18" spans="1:21" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
@@ -2215,22 +2212,22 @@
       <c r="E18" s="24">
         <v>0</v>
       </c>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="56"/>
-      <c r="J18" s="62"/>
-      <c r="K18" s="62"/>
-      <c r="L18" s="62"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="62"/>
-      <c r="O18" s="62"/>
-      <c r="P18" s="62"/>
-      <c r="Q18" s="56"/>
-      <c r="R18" s="62"/>
-      <c r="S18" s="62"/>
-      <c r="T18" s="62"/>
-      <c r="U18" s="56"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
+      <c r="J18" s="44"/>
+      <c r="K18" s="44"/>
+      <c r="L18" s="44"/>
+      <c r="M18" s="45"/>
+      <c r="N18" s="44"/>
+      <c r="O18" s="44"/>
+      <c r="P18" s="44"/>
+      <c r="Q18" s="45"/>
+      <c r="R18" s="44"/>
+      <c r="S18" s="44"/>
+      <c r="T18" s="44"/>
+      <c r="U18" s="45"/>
     </row>
     <row r="19" spans="1:21" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
@@ -2248,22 +2245,22 @@
       <c r="E19" s="28">
         <v>1</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="58"/>
-      <c r="J19" s="57"/>
-      <c r="K19" s="57"/>
-      <c r="L19" s="57"/>
-      <c r="M19" s="58"/>
-      <c r="N19" s="57"/>
-      <c r="O19" s="57"/>
-      <c r="P19" s="57"/>
-      <c r="Q19" s="58"/>
-      <c r="R19" s="57"/>
-      <c r="S19" s="57"/>
-      <c r="T19" s="57"/>
-      <c r="U19" s="58"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="47"/>
+      <c r="J19" s="46"/>
+      <c r="K19" s="46"/>
+      <c r="L19" s="46"/>
+      <c r="M19" s="47"/>
+      <c r="N19" s="46"/>
+      <c r="O19" s="46"/>
+      <c r="P19" s="46"/>
+      <c r="Q19" s="47"/>
+      <c r="R19" s="46"/>
+      <c r="S19" s="46"/>
+      <c r="T19" s="46"/>
+      <c r="U19" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -2287,7 +2284,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.5546875" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2302,38 +2299,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="43" t="s">
+      <c r="A1" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="43" t="s">
+      <c r="B1" s="57"/>
+      <c r="C1" s="57"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="45"/>
+      <c r="F1" s="57"/>
+      <c r="G1" s="57"/>
+      <c r="H1" s="58"/>
     </row>
     <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="40"/>
+      <c r="A2" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="53"/>
       <c r="C2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="40"/>
+      <c r="E2" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="53"/>
       <c r="G2" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="54" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2345,9 +2342,9 @@
         <v>22</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>51</v>
-      </c>
-      <c r="D3" s="42"/>
+        <v>50</v>
+      </c>
+      <c r="D3" s="55"/>
       <c r="E3" s="32" t="s">
         <v>21</v>
       </c>
@@ -2355,9 +2352,9 @@
         <v>22</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="H3" s="42"/>
+        <v>51</v>
+      </c>
+      <c r="H3" s="55"/>
     </row>
     <row r="4" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="33">
@@ -2464,38 +2461,38 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="43" t="s">
+      <c r="A8" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="43" t="s">
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+      <c r="D8" s="58"/>
+      <c r="E8" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="F8" s="44"/>
-      <c r="G8" s="44"/>
-      <c r="H8" s="45"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="57"/>
+      <c r="H8" s="58"/>
     </row>
     <row r="9" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9" s="40"/>
+      <c r="A9" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="53"/>
       <c r="C9" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="54" t="s">
         <v>24</v>
       </c>
-      <c r="E9" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="F9" s="40"/>
+      <c r="E9" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="53"/>
       <c r="G9" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="H9" s="41" t="s">
+      <c r="H9" s="54" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2507,9 +2504,9 @@
         <v>22</v>
       </c>
       <c r="C10" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="D10" s="42"/>
+        <v>52</v>
+      </c>
+      <c r="D10" s="55"/>
       <c r="E10" s="32" t="s">
         <v>21</v>
       </c>
@@ -2517,9 +2514,9 @@
         <v>22</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="H10" s="42"/>
+        <v>53</v>
+      </c>
+      <c r="H10" s="55"/>
     </row>
     <row r="11" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="33">
@@ -2622,7 +2619,7 @@
         <v>38</v>
       </c>
       <c r="H14" s="37" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
     </row>
   </sheetData>
@@ -2660,32 +2657,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="52"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="61"/>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
+      <c r="A2" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
@@ -3022,12 +3019,12 @@
       <c r="E14" s="27">
         <v>0</v>
       </c>
-      <c r="F14" s="53" t="s">
+      <c r="F14" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="54"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="43"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
@@ -3045,10 +3042,10 @@
       <c r="E15" s="24">
         <v>1</v>
       </c>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="56"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
@@ -3066,10 +3063,10 @@
       <c r="E16" s="24">
         <v>0</v>
       </c>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="56"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
@@ -3087,10 +3084,10 @@
       <c r="E17" s="24">
         <v>1</v>
       </c>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="56"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
@@ -3108,10 +3105,10 @@
       <c r="E18" s="24">
         <v>0</v>
       </c>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="56"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
@@ -3129,10 +3126,10 @@
       <c r="E19" s="28">
         <v>1</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="58"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3161,32 +3158,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="52"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="61"/>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
+      <c r="A2" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
@@ -3523,12 +3520,12 @@
       <c r="E14" s="27">
         <v>0</v>
       </c>
-      <c r="F14" s="53" t="s">
+      <c r="F14" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="54"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="43"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
@@ -3546,10 +3543,10 @@
       <c r="E15" s="24">
         <v>1</v>
       </c>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="56"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
@@ -3567,10 +3564,10 @@
       <c r="E16" s="24">
         <v>0</v>
       </c>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="56"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
@@ -3588,10 +3585,10 @@
       <c r="E17" s="24">
         <v>1</v>
       </c>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="56"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
@@ -3609,10 +3606,10 @@
       <c r="E18" s="24">
         <v>0</v>
       </c>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="56"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
@@ -3630,10 +3627,10 @@
       <c r="E19" s="28">
         <v>1</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="58"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -3662,32 +3659,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="52"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="61"/>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
+      <c r="A2" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
@@ -4024,12 +4021,12 @@
       <c r="E14" s="27">
         <v>0</v>
       </c>
-      <c r="F14" s="53" t="s">
+      <c r="F14" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="54"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="43"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
@@ -4047,10 +4044,10 @@
       <c r="E15" s="24">
         <v>1</v>
       </c>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="56"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
@@ -4068,10 +4065,10 @@
       <c r="E16" s="24">
         <v>0</v>
       </c>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="56"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
@@ -4089,10 +4086,10 @@
       <c r="E17" s="24">
         <v>1</v>
       </c>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="56"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
@@ -4110,10 +4107,10 @@
       <c r="E18" s="24">
         <v>0</v>
       </c>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="56"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
@@ -4131,10 +4128,10 @@
       <c r="E19" s="28">
         <v>1</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="58"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -4163,32 +4160,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="50" t="s">
+      <c r="A1" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="51"/>
-      <c r="C1" s="51"/>
-      <c r="D1" s="51"/>
-      <c r="E1" s="51"/>
-      <c r="F1" s="51"/>
-      <c r="G1" s="51"/>
-      <c r="H1" s="51"/>
-      <c r="I1" s="52"/>
+      <c r="B1" s="60"/>
+      <c r="C1" s="60"/>
+      <c r="D1" s="60"/>
+      <c r="E1" s="60"/>
+      <c r="F1" s="60"/>
+      <c r="G1" s="60"/>
+      <c r="H1" s="60"/>
+      <c r="I1" s="61"/>
     </row>
     <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="46"/>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="47" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="49"/>
+      <c r="A2" s="51" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="52"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="13" t="s">
@@ -4525,12 +4522,12 @@
       <c r="E14" s="27">
         <v>0</v>
       </c>
-      <c r="F14" s="53" t="s">
+      <c r="F14" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="54"/>
+      <c r="G14" s="42"/>
+      <c r="H14" s="42"/>
+      <c r="I14" s="43"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="8">
@@ -4548,10 +4545,10 @@
       <c r="E15" s="24">
         <v>1</v>
       </c>
-      <c r="F15" s="55"/>
-      <c r="G15" s="55"/>
-      <c r="H15" s="55"/>
-      <c r="I15" s="56"/>
+      <c r="F15" s="44"/>
+      <c r="G15" s="44"/>
+      <c r="H15" s="44"/>
+      <c r="I15" s="45"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="8">
@@ -4569,10 +4566,10 @@
       <c r="E16" s="24">
         <v>0</v>
       </c>
-      <c r="F16" s="55"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="55"/>
-      <c r="I16" s="56"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="8">
@@ -4590,10 +4587,10 @@
       <c r="E17" s="24">
         <v>1</v>
       </c>
-      <c r="F17" s="55"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="55"/>
-      <c r="I17" s="56"/>
+      <c r="F17" s="44"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="44"/>
+      <c r="I17" s="45"/>
     </row>
     <row r="18" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="8">
@@ -4611,10 +4608,10 @@
       <c r="E18" s="24">
         <v>0</v>
       </c>
-      <c r="F18" s="55"/>
-      <c r="G18" s="55"/>
-      <c r="H18" s="55"/>
-      <c r="I18" s="56"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="44"/>
+      <c r="H18" s="44"/>
+      <c r="I18" s="45"/>
     </row>
     <row r="19" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="9">
@@ -4632,10 +4629,10 @@
       <c r="E19" s="28">
         <v>1</v>
       </c>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="58"/>
+      <c r="F19" s="46"/>
+      <c r="G19" s="46"/>
+      <c r="H19" s="46"/>
+      <c r="I19" s="47"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>